<commit_message>
got loops kinda working
</commit_message>
<xml_diff>
--- a/test/templates/t3.xlsx
+++ b/test/templates/t3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Systems\xlsx-template\test\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E513B0B4-4AF9-45EE-AC25-8133FB7176BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F353953D-5829-46DB-8814-4DB0C5492D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,10 @@
     <t>{revision}</t>
   </si>
   <si>
-    <t>{table:planData.name}</t>
+    <t>{#planData.name}</t>
   </si>
   <si>
-    <t>{table:planData.role.name}</t>
+    <t>{#planData.role.name}</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
   <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>